<commit_message>
remove East Asia summary table
</commit_message>
<xml_diff>
--- a/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
+++ b/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic Analysis\QSYSpheroidsStudy\analysis\data\derived_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Downloads/QSY-Spheroids-Study/analysis/data/derived_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B420E69B-1827-43A0-BA01-309E593BF76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963AF073-850C-6C42-A9EE-CA20F09EC8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$43</definedName>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="73">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -278,84 +277,6 @@
   </si>
   <si>
     <t>QSY_A_0576</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>core type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unidirectional</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mlutifacial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bidirectional</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>centripetal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lava</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>dolomite</t>
-  </si>
-  <si>
-    <t>chert</t>
-  </si>
-  <si>
-    <t>weight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>length</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>width</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thickness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>polyhedron</t>
-  </si>
-  <si>
-    <t>subspheroid/spheroid</t>
-  </si>
-  <si>
-    <t>multifacial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -405,20 +326,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -427,7 +348,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -435,7 +356,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -443,14 +364,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -493,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -518,13 +439,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -532,7 +450,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -548,7 +466,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -846,33 +764,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D83CAE-D6B4-4386-A76F-E7D2B066338F}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" customHeight="1" thickBot="1">
+    <row r="1" spans="1:9" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -881,16 +799,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -907,16 +825,16 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="9">
+        <v>71</v>
+      </c>
+      <c r="G2" s="8">
         <v>0.86583878077459997</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>1.0202955009007799</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -935,14 +853,14 @@
       <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0.826994369477283</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>1.0427844090165399</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -961,14 +879,14 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.82553180591715303</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>1.07957120332497</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
@@ -987,14 +905,14 @@
       <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.80913134961550304</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>1.04957579148573</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1013,14 +931,14 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0.79883004524914303</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>1.05439890058428</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1039,14 +957,14 @@
       <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>0.80323641292673098</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>1.0390231881816401</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1063,16 +981,16 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="9">
+        <v>67</v>
+      </c>
+      <c r="G8" s="8">
         <v>0.91667152267275898</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>1.01039006872008</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1091,14 +1009,14 @@
       <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>0.88074504652137997</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>1.0248097727054499</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1115,19 +1033,19 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="9">
+        <v>66</v>
+      </c>
+      <c r="G10" s="8">
         <v>0.89339881930575105</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>1.0171219342175599</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1146,17 +1064,17 @@
       <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0.84191948715112197</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>1.0424149452095499</v>
       </c>
       <c r="I11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1173,16 +1091,16 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="9">
+        <v>66</v>
+      </c>
+      <c r="G12" s="8">
         <v>0.86781159737379698</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>1.01993180730621</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1201,14 +1119,14 @@
       <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.86904570191028696</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>1.0271441801932499</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1225,17 +1143,17 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="10">
+        <v>72</v>
+      </c>
+      <c r="G14" s="9">
         <v>0.91914375907962997</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>1.0128569569046999</v>
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1252,16 +1170,16 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="9">
+        <v>71</v>
+      </c>
+      <c r="G15" s="8">
         <v>0.87179809077771597</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>1.0227407691483601</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
@@ -1278,17 +1196,17 @@
         <v>25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="10">
+        <v>69</v>
+      </c>
+      <c r="G16" s="9">
         <v>0.89345869606101302</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <v>1.0108586624567799</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1305,19 +1223,19 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="9">
+        <v>67</v>
+      </c>
+      <c r="G17" s="8">
         <v>0.92740820588925599</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>1.0125298048507101</v>
       </c>
       <c r="I17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1336,14 +1254,14 @@
       <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>0.86753010246267503</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>1.0367929940665901</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1362,14 +1280,14 @@
       <c r="F19" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0.86067729256230097</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>1.0312513807869299</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -1388,14 +1306,14 @@
       <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>0.79551953142328402</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>1.07534470537947</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
@@ -1412,16 +1330,16 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="9">
+        <v>66</v>
+      </c>
+      <c r="G21" s="8">
         <v>0.854708339976051</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>1.0189490023246699</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1438,17 +1356,17 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="10">
+        <v>66</v>
+      </c>
+      <c r="G22" s="9">
         <v>0.89677785094664098</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="9">
         <v>1.01123055465165</v>
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1465,19 +1383,19 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="10">
+        <v>69</v>
+      </c>
+      <c r="G23" s="9">
         <v>0.90112023234401095</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="9">
         <v>1.0114625047224299</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -1496,15 +1414,15 @@
       <c r="F24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <v>0.89114064489367595</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="9">
         <v>1.0300395956189301</v>
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
@@ -1523,17 +1441,17 @@
       <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <v>0.86881976214962997</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <v>1.03117582770317</v>
       </c>
       <c r="I25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1549,18 +1467,18 @@
       <c r="E26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="10">
+      <c r="F26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="9">
         <v>0.87794630741784496</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="9">
         <v>1.01078651909895</v>
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
@@ -1577,19 +1495,19 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="9">
+        <v>71</v>
+      </c>
+      <c r="G27" s="8">
         <v>0.87570822074554999</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <v>1.02769700500226</v>
       </c>
       <c r="I27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1606,19 +1524,19 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="9">
+        <v>71</v>
+      </c>
+      <c r="G28" s="8">
         <v>0.90213221519950204</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <v>1.0165340520897299</v>
       </c>
       <c r="I28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
@@ -1635,17 +1553,17 @@
         <v>18</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="10">
+        <v>66</v>
+      </c>
+      <c r="G29" s="9">
         <v>0.92724171208478101</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="9">
         <v>1.0104906072626301</v>
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1664,17 +1582,17 @@
       <c r="F30" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="8">
         <v>0.82036095381129903</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="8">
         <v>1.0400019342068001</v>
       </c>
       <c r="I30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>47</v>
       </c>
@@ -1691,17 +1609,17 @@
         <v>25</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31" s="10">
+        <v>69</v>
+      </c>
+      <c r="G31" s="9">
         <v>0.90451693424286705</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31" s="9">
         <v>1.0113858172997301</v>
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>48</v>
       </c>
@@ -1718,17 +1636,17 @@
         <v>18</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" s="10">
+        <v>70</v>
+      </c>
+      <c r="G32" s="9">
         <v>0.90670636339442701</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H32" s="9">
         <v>1.0091197553155</v>
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
@@ -1745,17 +1663,17 @@
         <v>18</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="10">
+        <v>69</v>
+      </c>
+      <c r="G33" s="9">
         <v>0.93768376635683703</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H33" s="9">
         <v>1.00438246002945</v>
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>59</v>
       </c>
@@ -1772,17 +1690,17 @@
         <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="10">
+        <v>66</v>
+      </c>
+      <c r="G34" s="9">
         <v>0.91518809189496197</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H34" s="9">
         <v>1.0147381894682099</v>
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>50</v>
       </c>
@@ -1799,19 +1717,19 @@
         <v>25</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G35" s="10">
+        <v>72</v>
+      </c>
+      <c r="G35" s="9">
         <v>0.90212613413444998</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H35" s="9">
         <v>1.02041757098209</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13.2" customHeight="1">
+    <row r="36" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
@@ -1828,16 +1746,16 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
-      </c>
-      <c r="G36" s="9">
+        <v>72</v>
+      </c>
+      <c r="G36" s="8">
         <v>0.879131059248073</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="8">
         <v>1.0188914423940501</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="13.2" customHeight="1">
+    <row r="37" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -1854,19 +1772,19 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="9">
+        <v>65</v>
+      </c>
+      <c r="G37" s="8">
         <v>0.88580503990772097</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="8">
         <v>1.0242801421349601</v>
       </c>
       <c r="I37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1885,17 +1803,17 @@
       <c r="F38" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="8">
         <v>0.86311083380900899</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="8">
         <v>1.02448645054968</v>
       </c>
       <c r="I38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -1912,16 +1830,16 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="9">
+        <v>71</v>
+      </c>
+      <c r="G39" s="8">
         <v>0.89924394729934098</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="8">
         <v>1.0236440593158</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
@@ -1940,14 +1858,14 @@
       <c r="F40" t="s">
         <v>26</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="8">
         <v>0.86886780203928704</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="8">
         <v>1.02652473430849</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
@@ -1964,17 +1882,17 @@
         <v>25</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G41" s="10">
+        <v>72</v>
+      </c>
+      <c r="G41" s="9">
         <v>0.90450780877599701</v>
       </c>
-      <c r="H41" s="10">
+      <c r="H41" s="9">
         <v>1.01614124668183</v>
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -1991,16 +1909,16 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="9">
+        <v>65</v>
+      </c>
+      <c r="G42" s="8">
         <v>0.85898571053543105</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="8">
         <v>1.05274697320487</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -2017,12 +1935,12 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="9">
+        <v>71</v>
+      </c>
+      <c r="G43" s="8">
         <v>0.85783073585724501</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="8">
         <v>1.02041967166138</v>
       </c>
       <c r="I43" t="s">
@@ -2035,216 +1953,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A1CFE-EE35-4687-A7B2-150113A858EC}">
-  <dimension ref="A1:J23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
-  <cols>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates of text and figures
</commit_message>
<xml_diff>
--- a/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
+++ b/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic Analysis\QSYSpheroidsStudy\analysis\data\derived_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic_Analysis\QSYSpheroidsStudy\analysis\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BF89D7-6090-49CD-84D8-CBE2FCCF7E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B0A36-F395-4052-AC7C-9AEBECDC8084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31845" yWindow="1125" windowWidth="23010" windowHeight="12210" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="97">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,9 +366,6 @@
     <t>Blank type</t>
   </si>
   <si>
-    <t>Blank morphology</t>
-  </si>
-  <si>
     <t>Final morphology</t>
   </si>
   <si>
@@ -390,6 +387,30 @@
   </si>
   <si>
     <t>Ellipsoid or box</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rock_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lava</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other-quartz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other-quartzite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dolomite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +421,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +469,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -486,7 +518,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -523,7 +555,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -843,14 +890,14 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
     <col min="6" max="6" width="19.44140625" customWidth="1"/>
@@ -861,14 +908,14 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -880,7 +927,7 @@
         <v>82</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>38</v>
@@ -890,11 +937,11 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -903,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="8">
         <v>0.86583878077459997</v>
@@ -916,11 +963,11 @@
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -942,11 +989,11 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -968,11 +1015,11 @@
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -994,11 +1041,11 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1020,11 +1067,11 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1046,11 +1093,11 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1058,8 +1105,8 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>88</v>
+      <c r="F8" t="s">
+        <v>87</v>
       </c>
       <c r="G8" s="8">
         <v>0.91667152267275898</v>
@@ -1072,8 +1119,8 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
+      <c r="B9" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1098,11 +1145,11 @@
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
         <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1110,8 +1157,8 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>88</v>
+      <c r="F10" t="s">
+        <v>87</v>
       </c>
       <c r="G10" s="8">
         <v>0.89339881930575105</v>
@@ -1127,11 +1174,11 @@
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1156,11 +1203,11 @@
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
         <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -1168,8 +1215,8 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>88</v>
+      <c r="F12" t="s">
+        <v>87</v>
       </c>
       <c r="G12" s="8">
         <v>0.86781159737379698</v>
@@ -1182,8 +1229,8 @@
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
+      <c r="B13" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1208,8 +1255,8 @@
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
+      <c r="B14" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1221,7 +1268,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" s="9">
         <v>0.91914375907962997</v>
@@ -1235,11 +1282,11 @@
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1248,7 +1295,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" s="8">
         <v>0.87179809077771597</v>
@@ -1261,11 +1308,11 @@
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
@@ -1274,7 +1321,7 @@
         <v>25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="9">
         <v>0.89345869606101302</v>
@@ -1288,11 +1335,11 @@
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
         <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1300,8 +1347,8 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>88</v>
+      <c r="F17" t="s">
+        <v>87</v>
       </c>
       <c r="G17" s="8">
         <v>0.92740820588925599</v>
@@ -1317,11 +1364,11 @@
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -1343,8 +1390,8 @@
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
+      <c r="B19" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1369,11 +1416,11 @@
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -1395,8 +1442,8 @@
       <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
+      <c r="B21" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1407,8 +1454,8 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>88</v>
+      <c r="F21" t="s">
+        <v>87</v>
       </c>
       <c r="G21" s="8">
         <v>0.854708339976051</v>
@@ -1421,11 +1468,11 @@
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
@@ -1434,7 +1481,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="9">
         <v>0.89677785094664098</v>
@@ -1448,11 +1495,11 @@
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -1461,7 +1508,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" s="9">
         <v>0.90112023234401095</v>
@@ -1477,11 +1524,11 @@
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
@@ -1504,11 +1551,11 @@
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
         <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -1533,8 +1580,8 @@
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
+      <c r="B26" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1546,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" s="9">
         <v>0.87794630741784496</v>
@@ -1560,11 +1607,11 @@
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
         <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1573,7 +1620,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" s="8">
         <v>0.87570822074554999</v>
@@ -1589,11 +1636,11 @@
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
         <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1602,7 +1649,7 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" s="8">
         <v>0.90213221519950204</v>
@@ -1618,11 +1665,11 @@
       <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>24</v>
@@ -1631,7 +1678,7 @@
         <v>18</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" s="9">
         <v>0.92724171208478101</v>
@@ -1645,11 +1692,11 @@
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
         <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1674,11 +1721,11 @@
       <c r="A31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>7</v>
@@ -1687,7 +1734,7 @@
         <v>25</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" s="9">
         <v>0.90451693424286705</v>
@@ -1701,11 +1748,11 @@
       <c r="A32" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>24</v>
@@ -1714,7 +1761,7 @@
         <v>18</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G32" s="9">
         <v>0.90670636339442701</v>
@@ -1728,8 +1775,8 @@
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
+      <c r="B33" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1741,7 +1788,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="9">
         <v>0.93768376635683703</v>
@@ -1755,11 +1802,11 @@
       <c r="A34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>24</v>
@@ -1768,7 +1815,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="9">
         <v>0.91518809189496197</v>
@@ -1778,32 +1825,32 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:9" s="13" customFormat="1">
+      <c r="A35" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="E35" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="14">
         <v>0.90212613413444998</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="14">
         <v>1.02041757098209</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1811,11 +1858,11 @@
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
         <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -1824,7 +1871,7 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36" s="8">
         <v>0.879131059248073</v>
@@ -1837,11 +1884,11 @@
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
         <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1850,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G37" s="8">
         <v>0.88580503990772097</v>
@@ -1866,11 +1913,11 @@
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
         <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -1895,11 +1942,11 @@
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
         <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
@@ -1908,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G39" s="8">
         <v>0.89924394729934098</v>
@@ -1921,11 +1968,11 @@
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
         <v>12</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1947,11 +1994,11 @@
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>9</v>
@@ -1960,7 +2007,7 @@
         <v>25</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G41" s="9">
         <v>0.90450780877599701</v>
@@ -1974,11 +2021,11 @@
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" t="s">
         <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1987,7 +2034,7 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G42" s="8">
         <v>0.85898571053543105</v>
@@ -2000,11 +2047,11 @@
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s">
         <v>12</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -2013,7 +2060,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G43" s="8">
         <v>0.85783073585724501</v>

</xml_diff>

<commit_message>
many changes to get the Python workflow running on WSL ubuntu
</commit_message>
<xml_diff>
--- a/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
+++ b/analysis/data/derived_data/core_typology_morphological_parameters.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic_Analysis\QSYSpheroidsStudy\analysis\data\derived_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QSY-Spheroids-Study\analysis\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEFA80A-70F2-450F-8139-DE364103F7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC488B0-A63F-4371-AC29-999615F28875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
+    <workbookView xWindow="1290" yWindow="3315" windowWidth="13995" windowHeight="11835" xr2:uid="{55A32788-9AC2-4441-A160-4671F3C53985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="74">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -280,10 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Sphericity       </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Blank type</t>
   </si>
   <si>
@@ -291,10 +287,6 @@
   </si>
   <si>
     <t>Discoid-like</t>
-  </si>
-  <si>
-    <t>SHE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Sphere or rounded cube</t>
@@ -339,21 +331,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00000"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -362,7 +351,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -370,7 +359,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -378,14 +367,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -393,13 +382,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -441,7 +430,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -466,12 +455,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -484,21 +467,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,9 +485,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -554,7 +525,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -660,7 +631,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -802,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -810,35 +781,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D83CAE-D6B4-4386-A76F-E7D2B066338F}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.9" customHeight="1" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>70</v>
+      <c r="B1" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -847,21 +817,15 @@
         <v>1</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>71</v>
+      <c r="B2" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -873,21 +837,15 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0.86583878077459997</v>
-      </c>
-      <c r="H2" s="8">
-        <v>1.0202955009007799</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>72</v>
+      <c r="B3" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -901,19 +859,13 @@
       <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="8">
-        <v>0.826994369477283</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1.0427844090165399</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>71</v>
+      <c r="B4" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -927,19 +879,13 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8">
-        <v>0.82553180591715303</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1.07957120332497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>71</v>
+      <c r="B5" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -953,19 +899,13 @@
       <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8">
-        <v>0.80913134961550304</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1.04957579148573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>73</v>
+      <c r="B6" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -979,19 +919,13 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8">
-        <v>0.79883004524914303</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1.05439890058428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>73</v>
+      <c r="B7" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1005,19 +939,13 @@
       <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="8">
-        <v>0.80323641292673098</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1.0390231881816401</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>71</v>
+      <c r="B8" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -1029,22 +957,16 @@
         <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0.91667152267275898</v>
-      </c>
-      <c r="H8" s="9">
-        <v>1.01039006872008</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>71</v>
+      <c r="B9" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1058,19 +980,13 @@
       <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="8">
-        <v>0.88074504652137997</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1.0248097727054499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>74</v>
+      <c r="B10" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1082,24 +998,18 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.89339881930575105</v>
-      </c>
-      <c r="H10" s="8">
-        <v>1.0171219342175599</v>
-      </c>
-      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>71</v>
+      <c r="B11" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1113,22 +1023,16 @@
       <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="8">
-        <v>0.84191948715112197</v>
-      </c>
-      <c r="H11" s="8">
-        <v>1.0424149452095499</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>71</v>
+      <c r="B12" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1140,21 +1044,15 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0.86781159737379698</v>
-      </c>
-      <c r="H12" s="8">
-        <v>1.01993180730621</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>71</v>
+      <c r="B13" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1168,19 +1066,13 @@
       <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="8">
-        <v>0.86904570191028696</v>
-      </c>
-      <c r="H13" s="8">
-        <v>1.0271441801932499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>71</v>
+      <c r="B14" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1192,22 +1084,16 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0.91914375907962997</v>
-      </c>
-      <c r="H14" s="9">
-        <v>1.0128569569046999</v>
-      </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>73</v>
+      <c r="B15" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1219,21 +1105,15 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0.87179809077771597</v>
-      </c>
-      <c r="H15" s="8">
-        <v>1.0227407691483601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>71</v>
+      <c r="B16" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -1245,22 +1125,16 @@
         <v>25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0.89345869606101302</v>
-      </c>
-      <c r="H16" s="9">
-        <v>1.0108586624567799</v>
-      </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>71</v>
+      <c r="B17" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1272,24 +1146,18 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="8">
-        <v>0.92740820588925599</v>
-      </c>
-      <c r="H17" s="8">
-        <v>1.0125298048507101</v>
-      </c>
-      <c r="I17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>75</v>
+      <c r="B18" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1303,19 +1171,13 @@
       <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="8">
-        <v>0.86753010246267503</v>
-      </c>
-      <c r="H18" s="8">
-        <v>1.0367929940665901</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>71</v>
+      <c r="B19" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1329,19 +1191,13 @@
       <c r="F19" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="8">
-        <v>0.86067729256230097</v>
-      </c>
-      <c r="H19" s="8">
-        <v>1.0312513807869299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>71</v>
+      <c r="B20" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1355,19 +1211,13 @@
       <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="8">
-        <v>0.79551953142328402</v>
-      </c>
-      <c r="H20" s="8">
-        <v>1.07534470537947</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>71</v>
+      <c r="B21" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1379,21 +1229,15 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0.854708339976051</v>
-      </c>
-      <c r="H21" s="8">
-        <v>1.0189490023246699</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>75</v>
+      <c r="B22" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1405,22 +1249,16 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="9">
-        <v>0.89677785094664098</v>
-      </c>
-      <c r="H22" s="9">
-        <v>1.01123055465165</v>
-      </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>71</v>
+      <c r="B23" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
@@ -1432,51 +1270,38 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.90112023234401095</v>
-      </c>
-      <c r="H23" s="9">
-        <v>1.0114625047224299</v>
-      </c>
-      <c r="I23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="17">
-        <v>0.89114064489367595</v>
-      </c>
-      <c r="H24" s="17">
-        <v>1.0300395956189301</v>
-      </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>71</v>
+      <c r="B25" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1490,22 +1315,16 @@
       <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="8">
-        <v>0.86881976214962997</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1.03117582770317</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="G25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>71</v>
+      <c r="B26" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1516,23 +1335,17 @@
       <c r="E26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0.87794630741784496</v>
-      </c>
-      <c r="H26" s="9">
-        <v>1.01078651909895</v>
-      </c>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>71</v>
+      <c r="B27" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1544,24 +1357,18 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0.87570822074554999</v>
-      </c>
-      <c r="H27" s="8">
-        <v>1.02769700500226</v>
-      </c>
-      <c r="I27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>71</v>
+      <c r="B28" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1573,24 +1380,18 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0.90213221519950204</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1.0165340520897299</v>
-      </c>
-      <c r="I28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>75</v>
+      <c r="B29" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>4</v>
@@ -1602,22 +1403,16 @@
         <v>18</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0.92724171208478101</v>
-      </c>
-      <c r="H29" s="9">
-        <v>1.0104906072626301</v>
-      </c>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>75</v>
+      <c r="B30" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1631,22 +1426,16 @@
       <c r="F30" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="8">
-        <v>0.82036095381129903</v>
-      </c>
-      <c r="H30" s="8">
-        <v>1.0400019342068001</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="G30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>71</v>
+      <c r="B31" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
@@ -1658,22 +1447,16 @@
         <v>25</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="9">
-        <v>0.90451693424286705</v>
-      </c>
-      <c r="H31" s="9">
-        <v>1.0113858172997301</v>
-      </c>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>71</v>
+      <c r="B32" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
@@ -1685,22 +1468,16 @@
         <v>18</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="9">
-        <v>0.90670636339442701</v>
-      </c>
-      <c r="H32" s="9">
-        <v>1.0091197553155</v>
-      </c>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>71</v>
+      <c r="B33" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1712,22 +1489,16 @@
         <v>18</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" s="9">
-        <v>0.93768376635683703</v>
-      </c>
-      <c r="H33" s="9">
-        <v>1.00438246002945</v>
-      </c>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>71</v>
+      <c r="B34" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -1739,22 +1510,16 @@
         <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="9">
-        <v>0.91518809189496197</v>
-      </c>
-      <c r="H34" s="9">
-        <v>1.0147381894682099</v>
-      </c>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>71</v>
+      <c r="B35" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
@@ -1766,24 +1531,18 @@
         <v>25</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="9">
-        <v>0.90212613413444998</v>
-      </c>
-      <c r="H35" s="9">
-        <v>1.02041757098209</v>
-      </c>
-      <c r="I35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="13.15" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>71</v>
+      <c r="B36" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1795,21 +1554,15 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" s="8">
-        <v>0.879131059248073</v>
-      </c>
-      <c r="H36" s="8">
-        <v>1.0188914423940501</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="13.15" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>75</v>
+      <c r="B37" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1821,24 +1574,18 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="8">
-        <v>0.88580503990772097</v>
-      </c>
-      <c r="H37" s="8">
-        <v>1.0242801421349601</v>
-      </c>
-      <c r="I37" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>71</v>
+      <c r="B38" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1852,22 +1599,16 @@
       <c r="F38" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="8">
-        <v>0.86311083380900899</v>
-      </c>
-      <c r="H38" s="8">
-        <v>1.02448645054968</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="G38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>71</v>
+      <c r="B39" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1879,21 +1620,15 @@
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="8">
-        <v>0.89924394729934098</v>
-      </c>
-      <c r="H39" s="8">
-        <v>1.0236440593158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>75</v>
+      <c r="B40" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
@@ -1907,19 +1642,13 @@
       <c r="F40" t="s">
         <v>26</v>
       </c>
-      <c r="G40" s="8">
-        <v>0.86886780203928704</v>
-      </c>
-      <c r="H40" s="8">
-        <v>1.02652473430849</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>71</v>
+      <c r="B41" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>4</v>
@@ -1931,22 +1660,16 @@
         <v>25</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="9">
-        <v>0.90450780877599701</v>
-      </c>
-      <c r="H41" s="9">
-        <v>1.01614124668183</v>
-      </c>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>71</v>
+      <c r="B42" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1958,21 +1681,15 @@
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G42" s="8">
-        <v>0.85898571053543105</v>
-      </c>
-      <c r="H42" s="8">
-        <v>1.05274697320487</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>75</v>
+      <c r="B43" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -1984,15 +1701,9 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" s="8">
-        <v>0.85783073585724501</v>
-      </c>
-      <c r="H43" s="8">
-        <v>1.02041967166138</v>
-      </c>
-      <c r="I43" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>